<commit_message>
rebuild project Use Unirest to send request
</commit_message>
<xml_diff>
--- a/src/main/resources/requestFields.xlsx
+++ b/src/main/resources/requestFields.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t xml:space="preserve">country</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">АА0001АА</t>
+  </si>
+  <si>
+    <t xml:space="preserve">АВ2991АЕ</t>
   </si>
   <si>
     <t xml:space="preserve">Україна</t>
@@ -170,10 +173,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:J2"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,6 +235,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -251,7 +262,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E2:J2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,7 +304,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>41800</v>
@@ -308,16 +319,16 @@
         <v>101865281</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>10068</v>

</xml_diff>